<commit_message>
Fixed modbus outputs. Changed loads panel and removed alert templates from the name generator (fixed problems with that too)
</commit_message>
<xml_diff>
--- a/PanelCreator/src/Creator/textFiles/Io Names - March 10.xlsx
+++ b/PanelCreator/src/Creator/textFiles/Io Names - March 10.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="158">
   <si>
     <t>`Store`</t>
   </si>
@@ -458,9 +458,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Generate Alerts</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Alert Templates</t>
   </si>
   <si>
     <t xml:space="preserve"> Alert Time Frame</t>
@@ -574,6 +571,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -581,9 +581,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -890,11 +887,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O126"/>
+  <dimension ref="A1:N126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,17 +904,16 @@
     <col min="6" max="6" width="6.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="9.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>140</v>
       </c>
@@ -960,30 +956,26 @@
       <c r="N1" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="8"/>
-    </row>
-    <row r="3" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="9"/>
+    </row>
+    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1011,14 +1003,13 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4">
-        <v>0</v>
-      </c>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4"/>
       <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-    </row>
-    <row r="4" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1046,16 +1037,15 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4">
-        <v>1</v>
-      </c>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L4" s="4">
+        <v>1</v>
+      </c>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1083,18 +1073,17 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
+      <c r="L5" s="4">
+        <v>2</v>
+      </c>
       <c r="M5" s="4">
-        <v>2</v>
-      </c>
-      <c r="N5" s="4">
-        <v>1</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -1122,18 +1111,17 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
+      <c r="L6" s="4">
+        <v>2</v>
+      </c>
       <c r="M6" s="4">
-        <v>2</v>
-      </c>
-      <c r="N6" s="4">
-        <v>1</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -1161,18 +1149,17 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
+      <c r="L7" s="4">
+        <v>2</v>
+      </c>
       <c r="M7" s="4">
-        <v>2</v>
-      </c>
-      <c r="N7" s="4">
-        <v>1</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -1200,20 +1187,19 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
+      <c r="L8" s="4">
+        <v>2</v>
+      </c>
       <c r="M8" s="4">
-        <v>2</v>
-      </c>
-      <c r="N8" s="4">
-        <v>1</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B9" s="4">
         <v>1</v>
@@ -1239,18 +1225,17 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
+      <c r="L9" s="4">
+        <v>2</v>
+      </c>
       <c r="M9" s="4">
-        <v>2</v>
-      </c>
-      <c r="N9" s="4">
-        <v>1</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1278,14 +1263,13 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4">
-        <v>0</v>
-      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+      <c r="M10" s="4"/>
       <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-    </row>
-    <row r="11" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -1313,16 +1297,15 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4">
+      <c r="L11" s="4">
         <v>4</v>
       </c>
-      <c r="N11" s="4"/>
-      <c r="O11" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M11" s="4"/>
+      <c r="N11" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -1350,14 +1333,13 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4">
-        <v>0</v>
-      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4"/>
       <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-    </row>
-    <row r="13" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -1385,16 +1367,15 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4">
+      <c r="L13" s="4">
         <v>4</v>
       </c>
-      <c r="N13" s="4"/>
-      <c r="O13" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M13" s="4"/>
+      <c r="N13" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1422,18 +1403,17 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
+      <c r="L14" s="4">
+        <v>2</v>
+      </c>
       <c r="M14" s="4">
         <v>2</v>
       </c>
-      <c r="N14" s="4">
-        <v>2</v>
-      </c>
-      <c r="O14" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N14" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -1461,18 +1441,17 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
+      <c r="L15" s="4">
+        <v>2</v>
+      </c>
       <c r="M15" s="4">
         <v>2</v>
       </c>
-      <c r="N15" s="4">
-        <v>2</v>
-      </c>
-      <c r="O15" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N15" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
@@ -1500,18 +1479,17 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
+      <c r="L16" s="4">
+        <v>2</v>
+      </c>
       <c r="M16" s="4">
         <v>2</v>
       </c>
-      <c r="N16" s="4">
-        <v>2</v>
-      </c>
-      <c r="O16" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N16" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -1539,18 +1517,17 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
+      <c r="L17" s="4">
+        <v>2</v>
+      </c>
       <c r="M17" s="4">
         <v>2</v>
       </c>
-      <c r="N17" s="4">
-        <v>2</v>
-      </c>
-      <c r="O17" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N17" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
@@ -1578,18 +1555,17 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
+      <c r="L18" s="4">
+        <v>2</v>
+      </c>
       <c r="M18" s="4">
         <v>2</v>
       </c>
-      <c r="N18" s="4">
-        <v>2</v>
-      </c>
-      <c r="O18" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N18" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>29</v>
       </c>
@@ -1617,14 +1593,13 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4">
-        <v>0</v>
-      </c>
+      <c r="L19" s="4">
+        <v>0</v>
+      </c>
+      <c r="M19" s="4"/>
       <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-    </row>
-    <row r="20" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
@@ -1652,14 +1627,13 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4">
-        <v>0</v>
-      </c>
+      <c r="L20" s="4">
+        <v>0</v>
+      </c>
+      <c r="M20" s="4"/>
       <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-    </row>
-    <row r="21" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>31</v>
       </c>
@@ -1687,14 +1661,13 @@
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4">
-        <v>0</v>
-      </c>
+      <c r="L21" s="4">
+        <v>0</v>
+      </c>
+      <c r="M21" s="4"/>
       <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-    </row>
-    <row r="22" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
@@ -1722,16 +1695,15 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4">
-        <v>1</v>
-      </c>
-      <c r="N22" s="4"/>
-      <c r="O22" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L22" s="4">
+        <v>1</v>
+      </c>
+      <c r="M22" s="4"/>
+      <c r="N22" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
@@ -1759,16 +1731,15 @@
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4">
-        <v>1</v>
-      </c>
-      <c r="N23" s="4"/>
-      <c r="O23" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L23" s="4">
+        <v>1</v>
+      </c>
+      <c r="M23" s="4"/>
+      <c r="N23" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
@@ -1796,16 +1767,15 @@
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4">
-        <v>1</v>
-      </c>
-      <c r="N24" s="4"/>
-      <c r="O24" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L24" s="4">
+        <v>1</v>
+      </c>
+      <c r="M24" s="4"/>
+      <c r="N24" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
@@ -1833,16 +1803,15 @@
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4">
+      <c r="L25" s="4">
         <v>4</v>
       </c>
-      <c r="N25" s="4"/>
-      <c r="O25" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M25" s="4"/>
+      <c r="N25" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>37</v>
       </c>
@@ -1870,16 +1839,15 @@
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4">
+      <c r="L26" s="4">
         <v>4</v>
       </c>
-      <c r="N26" s="4"/>
-      <c r="O26" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M26" s="4"/>
+      <c r="N26" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>38</v>
       </c>
@@ -1907,16 +1875,15 @@
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4">
+      <c r="L27" s="4">
         <v>4</v>
       </c>
-      <c r="N27" s="4"/>
-      <c r="O27" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M27" s="4"/>
+      <c r="N27" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>39</v>
       </c>
@@ -1944,16 +1911,15 @@
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4">
+      <c r="L28" s="4">
         <v>4</v>
       </c>
-      <c r="N28" s="4"/>
-      <c r="O28" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M28" s="4"/>
+      <c r="N28" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>40</v>
       </c>
@@ -1981,16 +1947,15 @@
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4">
+      <c r="L29" s="4">
         <v>4</v>
       </c>
-      <c r="N29" s="4"/>
-      <c r="O29" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M29" s="4"/>
+      <c r="N29" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>41</v>
       </c>
@@ -2018,35 +1983,33 @@
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4">
+      <c r="L30" s="4">
         <v>4</v>
       </c>
-      <c r="N30" s="4"/>
-      <c r="O30" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-    </row>
-    <row r="32" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M30" s="4"/>
+      <c r="N30" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+    </row>
+    <row r="32" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>42</v>
       </c>
@@ -2074,16 +2037,15 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4">
+      <c r="L32" s="4">
         <v>4</v>
       </c>
-      <c r="N32" s="4"/>
-      <c r="O32" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M32" s="4"/>
+      <c r="N32" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>44</v>
       </c>
@@ -2111,16 +2073,15 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4">
+      <c r="L33" s="4">
         <v>4</v>
       </c>
-      <c r="N33" s="4"/>
-      <c r="O33" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M33" s="4"/>
+      <c r="N33" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>45</v>
       </c>
@@ -2148,18 +2109,17 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
+      <c r="L34" s="4">
+        <v>5</v>
+      </c>
       <c r="M34" s="4">
-        <v>5</v>
-      </c>
-      <c r="N34" s="4">
-        <v>1</v>
-      </c>
-      <c r="O34" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N34" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>47</v>
       </c>
@@ -2187,18 +2147,17 @@
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
+      <c r="L35" s="4">
+        <v>5</v>
+      </c>
       <c r="M35" s="4">
-        <v>5</v>
-      </c>
-      <c r="N35" s="4">
-        <v>1</v>
-      </c>
-      <c r="O35" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N35" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>49</v>
       </c>
@@ -2226,16 +2185,15 @@
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4">
+      <c r="L36" s="4">
         <v>4</v>
       </c>
-      <c r="N36" s="4"/>
-      <c r="O36" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M36" s="4"/>
+      <c r="N36" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>50</v>
       </c>
@@ -2263,18 +2221,17 @@
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
+      <c r="L37" s="4">
+        <v>5</v>
+      </c>
       <c r="M37" s="4">
-        <v>5</v>
-      </c>
-      <c r="N37" s="4">
-        <v>1</v>
-      </c>
-      <c r="O37" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N37" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>51</v>
       </c>
@@ -2302,18 +2259,17 @@
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
+      <c r="L38" s="4">
+        <v>5</v>
+      </c>
       <c r="M38" s="4">
-        <v>5</v>
-      </c>
-      <c r="N38" s="4">
-        <v>1</v>
-      </c>
-      <c r="O38" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N38" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>52</v>
       </c>
@@ -2341,16 +2297,15 @@
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4">
+      <c r="L39" s="4">
         <v>4</v>
       </c>
-      <c r="N39" s="4"/>
-      <c r="O39" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M39" s="4"/>
+      <c r="N39" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>53</v>
       </c>
@@ -2378,16 +2333,15 @@
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4">
+      <c r="L40" s="4">
         <v>4</v>
       </c>
-      <c r="N40" s="4"/>
-      <c r="O40" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M40" s="4"/>
+      <c r="N40" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>54</v>
       </c>
@@ -2415,14 +2369,13 @@
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4">
-        <v>0</v>
-      </c>
+      <c r="L41" s="4">
+        <v>0</v>
+      </c>
+      <c r="M41" s="4"/>
       <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-    </row>
-    <row r="42" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>55</v>
       </c>
@@ -2450,14 +2403,13 @@
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
-      <c r="M42" s="4">
-        <v>0</v>
-      </c>
+      <c r="L42" s="4">
+        <v>0</v>
+      </c>
+      <c r="M42" s="4"/>
       <c r="N42" s="4"/>
-      <c r="O42" s="4"/>
-    </row>
-    <row r="43" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>56</v>
       </c>
@@ -2485,14 +2437,13 @@
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
-      <c r="M43" s="4">
-        <v>0</v>
-      </c>
+      <c r="L43" s="4">
+        <v>0</v>
+      </c>
+      <c r="M43" s="4"/>
       <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
-    </row>
-    <row r="44" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>57</v>
       </c>
@@ -2520,14 +2471,13 @@
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="4">
-        <v>0</v>
-      </c>
+      <c r="L44" s="4">
+        <v>0</v>
+      </c>
+      <c r="M44" s="4"/>
       <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-    </row>
-    <row r="45" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>59</v>
       </c>
@@ -2555,14 +2505,13 @@
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
-      <c r="M45" s="4">
-        <v>0</v>
-      </c>
+      <c r="L45" s="4">
+        <v>0</v>
+      </c>
+      <c r="M45" s="4"/>
       <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
-    </row>
-    <row r="46" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>60</v>
       </c>
@@ -2590,18 +2539,17 @@
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
+      <c r="L46" s="4">
+        <v>5</v>
+      </c>
       <c r="M46" s="4">
-        <v>5</v>
-      </c>
-      <c r="N46" s="4">
-        <v>1</v>
-      </c>
-      <c r="O46" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N46" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>62</v>
       </c>
@@ -2629,14 +2577,13 @@
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4">
-        <v>0</v>
-      </c>
+      <c r="L47" s="4">
+        <v>0</v>
+      </c>
+      <c r="M47" s="4"/>
       <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-    </row>
-    <row r="48" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>63</v>
       </c>
@@ -2664,14 +2611,13 @@
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="4">
-        <v>0</v>
-      </c>
+      <c r="L48" s="4">
+        <v>0</v>
+      </c>
+      <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
-    </row>
-    <row r="49" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>64</v>
       </c>
@@ -2699,14 +2645,13 @@
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4">
-        <v>0</v>
-      </c>
+      <c r="L49" s="4">
+        <v>0</v>
+      </c>
+      <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-    </row>
-    <row r="50" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>66</v>
       </c>
@@ -2734,14 +2679,13 @@
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
-      <c r="L50" s="4"/>
-      <c r="M50" s="4">
-        <v>0</v>
-      </c>
+      <c r="L50" s="4">
+        <v>0</v>
+      </c>
+      <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="4"/>
-    </row>
-    <row r="51" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>67</v>
       </c>
@@ -2769,14 +2713,13 @@
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
-      <c r="L51" s="4"/>
-      <c r="M51" s="4">
-        <v>0</v>
-      </c>
+      <c r="L51" s="4">
+        <v>0</v>
+      </c>
+      <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="4"/>
-    </row>
-    <row r="52" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>68</v>
       </c>
@@ -2804,18 +2747,17 @@
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
-      <c r="L52" s="4"/>
+      <c r="L52" s="4">
+        <v>5</v>
+      </c>
       <c r="M52" s="4">
-        <v>5</v>
-      </c>
-      <c r="N52" s="4">
-        <v>1</v>
-      </c>
-      <c r="O52" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N52" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>69</v>
       </c>
@@ -2843,18 +2785,17 @@
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
-      <c r="L53" s="4"/>
+      <c r="L53" s="4">
+        <v>5</v>
+      </c>
       <c r="M53" s="4">
-        <v>5</v>
-      </c>
-      <c r="N53" s="4">
-        <v>1</v>
-      </c>
-      <c r="O53" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N53" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>70</v>
       </c>
@@ -2880,14 +2821,13 @@
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="4">
-        <v>0</v>
-      </c>
+      <c r="L54" s="4">
+        <v>0</v>
+      </c>
+      <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="4"/>
-    </row>
-    <row r="55" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>71</v>
       </c>
@@ -2913,14 +2853,13 @@
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="4">
-        <v>0</v>
-      </c>
+      <c r="L55" s="4">
+        <v>0</v>
+      </c>
+      <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="4"/>
-    </row>
-    <row r="56" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>72</v>
       </c>
@@ -2948,14 +2887,13 @@
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
-      <c r="M56" s="4">
-        <v>0</v>
-      </c>
+      <c r="L56" s="4">
+        <v>0</v>
+      </c>
+      <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="4"/>
-    </row>
-    <row r="57" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>73</v>
       </c>
@@ -2983,14 +2921,13 @@
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
-      <c r="L57" s="4"/>
-      <c r="M57" s="4">
-        <v>0</v>
-      </c>
+      <c r="L57" s="4">
+        <v>0</v>
+      </c>
+      <c r="M57" s="4"/>
       <c r="N57" s="4"/>
-      <c r="O57" s="4"/>
-    </row>
-    <row r="58" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>74</v>
       </c>
@@ -3018,18 +2955,17 @@
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
-      <c r="L58" s="4"/>
+      <c r="L58" s="4">
+        <v>5</v>
+      </c>
       <c r="M58" s="4">
-        <v>5</v>
-      </c>
-      <c r="N58" s="4">
-        <v>1</v>
-      </c>
-      <c r="O58" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N58" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>75</v>
       </c>
@@ -3057,18 +2993,17 @@
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
-      <c r="L59" s="4"/>
+      <c r="L59" s="4">
+        <v>5</v>
+      </c>
       <c r="M59" s="4">
-        <v>5</v>
-      </c>
-      <c r="N59" s="4">
-        <v>1</v>
-      </c>
-      <c r="O59" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N59" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>76</v>
       </c>
@@ -3096,16 +3031,15 @@
       <c r="I60" s="4"/>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
-      <c r="L60" s="4"/>
-      <c r="M60" s="4">
+      <c r="L60" s="4">
         <v>4</v>
       </c>
-      <c r="N60" s="4"/>
-      <c r="O60" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M60" s="4"/>
+      <c r="N60" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>77</v>
       </c>
@@ -3133,18 +3067,17 @@
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
-      <c r="L61" s="4"/>
+      <c r="L61" s="4">
+        <v>5</v>
+      </c>
       <c r="M61" s="4">
-        <v>5</v>
-      </c>
-      <c r="N61" s="4">
-        <v>1</v>
-      </c>
-      <c r="O61" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N61" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>78</v>
       </c>
@@ -3172,16 +3105,15 @@
       <c r="I62" s="4"/>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
-      <c r="L62" s="4"/>
-      <c r="M62" s="4">
+      <c r="L62" s="4">
         <v>4</v>
       </c>
-      <c r="N62" s="4"/>
-      <c r="O62" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M62" s="4"/>
+      <c r="N62" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>79</v>
       </c>
@@ -3209,18 +3141,17 @@
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
+      <c r="L63" s="4">
+        <v>5</v>
+      </c>
       <c r="M63" s="4">
-        <v>5</v>
-      </c>
-      <c r="N63" s="4">
-        <v>1</v>
-      </c>
-      <c r="O63" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N63" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>80</v>
       </c>
@@ -3248,16 +3179,15 @@
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
-      <c r="L64" s="4"/>
-      <c r="M64" s="4">
+      <c r="L64" s="4">
         <v>4</v>
       </c>
-      <c r="N64" s="4"/>
-      <c r="O64" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M64" s="4"/>
+      <c r="N64" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>81</v>
       </c>
@@ -3285,14 +3215,13 @@
       <c r="I65" s="4"/>
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
-      <c r="L65" s="4"/>
-      <c r="M65" s="4">
-        <v>0</v>
-      </c>
+      <c r="L65" s="4">
+        <v>0</v>
+      </c>
+      <c r="M65" s="4"/>
       <c r="N65" s="4"/>
-      <c r="O65" s="4"/>
-    </row>
-    <row r="66" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>82</v>
       </c>
@@ -3318,24 +3247,21 @@
         <v>1</v>
       </c>
       <c r="I66" s="4">
-        <v>11</v>
+        <v>300</v>
       </c>
       <c r="J66" s="4">
-        <v>300</v>
+        <v>2</v>
       </c>
       <c r="K66" s="4">
-        <v>2</v>
+        <v>115</v>
       </c>
       <c r="L66" s="4">
-        <v>115</v>
-      </c>
-      <c r="M66" s="4">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M66" s="4"/>
       <c r="N66" s="4"/>
-      <c r="O66" s="4"/>
-    </row>
-    <row r="67" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>83</v>
       </c>
@@ -3363,14 +3289,13 @@
       <c r="I67" s="4"/>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
-      <c r="L67" s="4"/>
-      <c r="M67" s="4">
-        <v>0</v>
-      </c>
+      <c r="L67" s="4">
+        <v>0</v>
+      </c>
+      <c r="M67" s="4"/>
       <c r="N67" s="4"/>
-      <c r="O67" s="4"/>
-    </row>
-    <row r="68" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>84</v>
       </c>
@@ -3398,14 +3323,13 @@
       <c r="I68" s="4"/>
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
-      <c r="L68" s="4"/>
-      <c r="M68" s="4">
-        <v>0</v>
-      </c>
+      <c r="L68" s="4">
+        <v>0</v>
+      </c>
+      <c r="M68" s="4"/>
       <c r="N68" s="4"/>
-      <c r="O68" s="4"/>
-    </row>
-    <row r="69" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>85</v>
       </c>
@@ -3433,14 +3357,13 @@
       <c r="I69" s="4"/>
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
-      <c r="L69" s="4"/>
-      <c r="M69" s="4">
-        <v>0</v>
-      </c>
+      <c r="L69" s="4">
+        <v>0</v>
+      </c>
+      <c r="M69" s="4"/>
       <c r="N69" s="4"/>
-      <c r="O69" s="4"/>
-    </row>
-    <row r="70" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>86</v>
       </c>
@@ -3468,14 +3391,13 @@
       <c r="I70" s="4"/>
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
-      <c r="L70" s="4"/>
-      <c r="M70" s="4">
-        <v>0</v>
-      </c>
+      <c r="L70" s="4">
+        <v>0</v>
+      </c>
+      <c r="M70" s="4"/>
       <c r="N70" s="4"/>
-      <c r="O70" s="4"/>
-    </row>
-    <row r="71" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>87</v>
       </c>
@@ -3503,14 +3425,13 @@
       <c r="I71" s="4"/>
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
-      <c r="L71" s="4"/>
-      <c r="M71" s="4">
-        <v>0</v>
-      </c>
+      <c r="L71" s="4">
+        <v>0</v>
+      </c>
+      <c r="M71" s="4"/>
       <c r="N71" s="4"/>
-      <c r="O71" s="4"/>
-    </row>
-    <row r="72" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>88</v>
       </c>
@@ -3538,14 +3459,13 @@
       <c r="I72" s="4"/>
       <c r="J72" s="4"/>
       <c r="K72" s="4"/>
-      <c r="L72" s="4"/>
-      <c r="M72" s="4">
-        <v>0</v>
-      </c>
+      <c r="L72" s="4">
+        <v>0</v>
+      </c>
+      <c r="M72" s="4"/>
       <c r="N72" s="4"/>
-      <c r="O72" s="4"/>
-    </row>
-    <row r="73" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>89</v>
       </c>
@@ -3573,14 +3493,13 @@
       <c r="I73" s="4"/>
       <c r="J73" s="4"/>
       <c r="K73" s="4"/>
-      <c r="L73" s="4"/>
-      <c r="M73" s="4">
-        <v>0</v>
-      </c>
+      <c r="L73" s="4">
+        <v>0</v>
+      </c>
+      <c r="M73" s="4"/>
       <c r="N73" s="4"/>
-      <c r="O73" s="4"/>
-    </row>
-    <row r="74" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>90</v>
       </c>
@@ -3608,14 +3527,13 @@
       <c r="I74" s="4"/>
       <c r="J74" s="4"/>
       <c r="K74" s="4"/>
-      <c r="L74" s="4"/>
-      <c r="M74" s="4">
-        <v>0</v>
-      </c>
+      <c r="L74" s="4">
+        <v>0</v>
+      </c>
+      <c r="M74" s="4"/>
       <c r="N74" s="4"/>
-      <c r="O74" s="4"/>
-    </row>
-    <row r="75" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>91</v>
       </c>
@@ -3643,14 +3561,13 @@
       <c r="I75" s="4"/>
       <c r="J75" s="4"/>
       <c r="K75" s="4"/>
-      <c r="L75" s="4"/>
-      <c r="M75" s="4">
-        <v>0</v>
-      </c>
+      <c r="L75" s="4">
+        <v>0</v>
+      </c>
+      <c r="M75" s="4"/>
       <c r="N75" s="4"/>
-      <c r="O75" s="4"/>
-    </row>
-    <row r="76" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>92</v>
       </c>
@@ -3678,14 +3595,13 @@
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
       <c r="K76" s="4"/>
-      <c r="L76" s="4"/>
-      <c r="M76" s="4">
-        <v>0</v>
-      </c>
+      <c r="L76" s="4">
+        <v>0</v>
+      </c>
+      <c r="M76" s="4"/>
       <c r="N76" s="4"/>
-      <c r="O76" s="4"/>
-    </row>
-    <row r="77" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>93</v>
       </c>
@@ -3713,14 +3629,13 @@
       <c r="I77" s="4"/>
       <c r="J77" s="4"/>
       <c r="K77" s="4"/>
-      <c r="L77" s="4"/>
-      <c r="M77" s="4">
-        <v>0</v>
-      </c>
+      <c r="L77" s="4">
+        <v>0</v>
+      </c>
+      <c r="M77" s="4"/>
       <c r="N77" s="4"/>
-      <c r="O77" s="4"/>
-    </row>
-    <row r="78" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>94</v>
       </c>
@@ -3748,14 +3663,13 @@
       <c r="I78" s="4"/>
       <c r="J78" s="4"/>
       <c r="K78" s="4"/>
-      <c r="L78" s="4"/>
-      <c r="M78" s="4">
-        <v>0</v>
-      </c>
+      <c r="L78" s="4">
+        <v>0</v>
+      </c>
+      <c r="M78" s="4"/>
       <c r="N78" s="4"/>
-      <c r="O78" s="4"/>
-    </row>
-    <row r="79" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>95</v>
       </c>
@@ -3783,14 +3697,13 @@
       <c r="I79" s="4"/>
       <c r="J79" s="4"/>
       <c r="K79" s="4"/>
-      <c r="L79" s="4"/>
-      <c r="M79" s="4">
-        <v>0</v>
-      </c>
+      <c r="L79" s="4">
+        <v>0</v>
+      </c>
+      <c r="M79" s="4"/>
       <c r="N79" s="4"/>
-      <c r="O79" s="4"/>
-    </row>
-    <row r="80" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>96</v>
       </c>
@@ -3818,14 +3731,13 @@
       <c r="I80" s="4"/>
       <c r="J80" s="4"/>
       <c r="K80" s="4"/>
-      <c r="L80" s="4"/>
-      <c r="M80" s="4">
-        <v>0</v>
-      </c>
+      <c r="L80" s="4">
+        <v>0</v>
+      </c>
+      <c r="M80" s="4"/>
       <c r="N80" s="4"/>
-      <c r="O80" s="4"/>
-    </row>
-    <row r="81" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>97</v>
       </c>
@@ -3853,14 +3765,13 @@
       <c r="I81" s="4"/>
       <c r="J81" s="4"/>
       <c r="K81" s="4"/>
-      <c r="L81" s="4"/>
-      <c r="M81" s="4">
-        <v>0</v>
-      </c>
+      <c r="L81" s="4">
+        <v>0</v>
+      </c>
+      <c r="M81" s="4"/>
       <c r="N81" s="4"/>
-      <c r="O81" s="4"/>
-    </row>
-    <row r="82" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>98</v>
       </c>
@@ -3888,16 +3799,15 @@
       <c r="I82" s="4"/>
       <c r="J82" s="4"/>
       <c r="K82" s="4"/>
-      <c r="L82" s="4"/>
-      <c r="M82" s="4">
-        <v>1</v>
-      </c>
-      <c r="N82" s="4"/>
-      <c r="O82" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L82" s="4">
+        <v>1</v>
+      </c>
+      <c r="M82" s="4"/>
+      <c r="N82" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>99</v>
       </c>
@@ -3925,16 +3835,15 @@
       <c r="I83" s="4"/>
       <c r="J83" s="4"/>
       <c r="K83" s="4"/>
-      <c r="L83" s="4"/>
-      <c r="M83" s="4">
-        <v>1</v>
-      </c>
-      <c r="N83" s="4"/>
-      <c r="O83" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L83" s="4">
+        <v>1</v>
+      </c>
+      <c r="M83" s="4"/>
+      <c r="N83" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>100</v>
       </c>
@@ -3962,16 +3871,15 @@
       <c r="I84" s="4"/>
       <c r="J84" s="4"/>
       <c r="K84" s="4"/>
-      <c r="L84" s="4"/>
-      <c r="M84" s="4">
-        <v>1</v>
-      </c>
-      <c r="N84" s="4"/>
-      <c r="O84" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L84" s="4">
+        <v>1</v>
+      </c>
+      <c r="M84" s="4"/>
+      <c r="N84" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>101</v>
       </c>
@@ -3999,16 +3907,15 @@
       <c r="I85" s="4"/>
       <c r="J85" s="4"/>
       <c r="K85" s="4"/>
-      <c r="L85" s="4"/>
-      <c r="M85" s="4">
+      <c r="L85" s="4">
         <v>4</v>
       </c>
-      <c r="N85" s="4"/>
-      <c r="O85" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M85" s="4"/>
+      <c r="N85" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>102</v>
       </c>
@@ -4036,16 +3943,15 @@
       <c r="I86" s="4"/>
       <c r="J86" s="4"/>
       <c r="K86" s="4"/>
-      <c r="L86" s="4"/>
-      <c r="M86" s="4">
+      <c r="L86" s="4">
         <v>4</v>
       </c>
-      <c r="N86" s="4"/>
-      <c r="O86" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M86" s="4"/>
+      <c r="N86" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>103</v>
       </c>
@@ -4073,16 +3979,15 @@
       <c r="I87" s="4"/>
       <c r="J87" s="4"/>
       <c r="K87" s="4"/>
-      <c r="L87" s="4"/>
-      <c r="M87" s="4">
+      <c r="L87" s="4">
         <v>4</v>
       </c>
-      <c r="N87" s="4"/>
-      <c r="O87" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="88" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M87" s="4"/>
+      <c r="N87" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>104</v>
       </c>
@@ -4110,16 +4015,15 @@
       <c r="I88" s="4"/>
       <c r="J88" s="4"/>
       <c r="K88" s="4"/>
-      <c r="L88" s="4"/>
-      <c r="M88" s="4">
+      <c r="L88" s="4">
         <v>4</v>
       </c>
-      <c r="N88" s="4"/>
-      <c r="O88" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="89" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M88" s="4"/>
+      <c r="N88" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>105</v>
       </c>
@@ -4147,18 +4051,17 @@
       <c r="I89" s="4"/>
       <c r="J89" s="4"/>
       <c r="K89" s="4"/>
-      <c r="L89" s="4"/>
+      <c r="L89" s="4">
+        <v>5</v>
+      </c>
       <c r="M89" s="4">
-        <v>5</v>
-      </c>
-      <c r="N89" s="4">
-        <v>1</v>
-      </c>
-      <c r="O89" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="90" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N89" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>106</v>
       </c>
@@ -4186,18 +4089,17 @@
       <c r="I90" s="4"/>
       <c r="J90" s="4"/>
       <c r="K90" s="4"/>
-      <c r="L90" s="4"/>
+      <c r="L90" s="4">
+        <v>2</v>
+      </c>
       <c r="M90" s="4">
         <v>2</v>
       </c>
-      <c r="N90" s="4">
-        <v>2</v>
-      </c>
-      <c r="O90" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N90" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>107</v>
       </c>
@@ -4225,18 +4127,17 @@
       <c r="I91" s="4"/>
       <c r="J91" s="4"/>
       <c r="K91" s="4"/>
-      <c r="L91" s="4"/>
+      <c r="L91" s="4">
+        <v>2</v>
+      </c>
       <c r="M91" s="4">
         <v>2</v>
       </c>
-      <c r="N91" s="4">
-        <v>2</v>
-      </c>
-      <c r="O91" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="92" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N91" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>108</v>
       </c>
@@ -4264,14 +4165,13 @@
       <c r="I92" s="4"/>
       <c r="J92" s="4"/>
       <c r="K92" s="4"/>
-      <c r="L92" s="4"/>
-      <c r="M92" s="4">
-        <v>0</v>
-      </c>
-      <c r="N92" s="4"/>
-      <c r="O92" s="5"/>
-    </row>
-    <row r="93" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L92" s="4">
+        <v>0</v>
+      </c>
+      <c r="M92" s="4"/>
+      <c r="N92" s="5"/>
+    </row>
+    <row r="93" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>109</v>
       </c>
@@ -4299,14 +4199,13 @@
       <c r="I93" s="4"/>
       <c r="J93" s="4"/>
       <c r="K93" s="4"/>
-      <c r="L93" s="4"/>
-      <c r="M93" s="4">
-        <v>0</v>
-      </c>
+      <c r="L93" s="4">
+        <v>0</v>
+      </c>
+      <c r="M93" s="4"/>
       <c r="N93" s="4"/>
-      <c r="O93" s="4"/>
-    </row>
-    <row r="94" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>110</v>
       </c>
@@ -4334,14 +4233,13 @@
       <c r="I94" s="4"/>
       <c r="J94" s="4"/>
       <c r="K94" s="4"/>
-      <c r="L94" s="4"/>
-      <c r="M94" s="4">
-        <v>0</v>
-      </c>
+      <c r="L94" s="4">
+        <v>0</v>
+      </c>
+      <c r="M94" s="4"/>
       <c r="N94" s="4"/>
-      <c r="O94" s="4"/>
-    </row>
-    <row r="95" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>111</v>
       </c>
@@ -4369,18 +4267,17 @@
       <c r="I95" s="4"/>
       <c r="J95" s="4"/>
       <c r="K95" s="4"/>
-      <c r="L95" s="4"/>
+      <c r="L95" s="4">
+        <v>5</v>
+      </c>
       <c r="M95" s="4">
-        <v>5</v>
-      </c>
-      <c r="N95" s="4">
-        <v>1</v>
-      </c>
-      <c r="O95" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="96" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N95" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>112</v>
       </c>
@@ -4408,18 +4305,17 @@
       <c r="I96" s="4"/>
       <c r="J96" s="4"/>
       <c r="K96" s="4"/>
-      <c r="L96" s="4"/>
+      <c r="L96" s="4">
+        <v>5</v>
+      </c>
       <c r="M96" s="4">
-        <v>5</v>
-      </c>
-      <c r="N96" s="4">
-        <v>1</v>
-      </c>
-      <c r="O96" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="97" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N96" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>113</v>
       </c>
@@ -4445,33 +4341,31 @@
       <c r="I97" s="4"/>
       <c r="J97" s="4"/>
       <c r="K97" s="4"/>
-      <c r="L97" s="4"/>
-      <c r="M97" s="4">
-        <v>0</v>
-      </c>
+      <c r="L97" s="4">
+        <v>0</v>
+      </c>
+      <c r="M97" s="4"/>
       <c r="N97" s="4"/>
-      <c r="O97" s="4"/>
-    </row>
-    <row r="98" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B98" s="9"/>
-      <c r="C98" s="9"/>
-      <c r="D98" s="9"/>
-      <c r="E98" s="9"/>
-      <c r="F98" s="9"/>
-      <c r="G98" s="9"/>
-      <c r="H98" s="9"/>
-      <c r="I98" s="9"/>
-      <c r="J98" s="9"/>
-      <c r="K98" s="9"/>
-      <c r="L98" s="9"/>
-      <c r="M98" s="9"/>
-      <c r="N98" s="9"/>
-      <c r="O98" s="9"/>
-    </row>
-    <row r="99" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B98" s="6"/>
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="6"/>
+      <c r="G98" s="6"/>
+      <c r="H98" s="6"/>
+      <c r="I98" s="6"/>
+      <c r="J98" s="6"/>
+      <c r="K98" s="6"/>
+      <c r="L98" s="6"/>
+      <c r="M98" s="6"/>
+      <c r="N98" s="6"/>
+    </row>
+    <row r="99" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>114</v>
       </c>
@@ -4499,14 +4393,13 @@
       <c r="I99" s="4"/>
       <c r="J99" s="4"/>
       <c r="K99" s="4"/>
-      <c r="L99" s="4"/>
-      <c r="M99" s="4">
-        <v>0</v>
-      </c>
+      <c r="L99" s="4">
+        <v>0</v>
+      </c>
+      <c r="M99" s="4"/>
       <c r="N99" s="4"/>
-      <c r="O99" s="4"/>
-    </row>
-    <row r="100" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>115</v>
       </c>
@@ -4532,14 +4425,13 @@
       <c r="I100" s="4"/>
       <c r="J100" s="4"/>
       <c r="K100" s="4"/>
-      <c r="L100" s="4"/>
-      <c r="M100" s="4">
-        <v>0</v>
-      </c>
+      <c r="L100" s="4">
+        <v>0</v>
+      </c>
+      <c r="M100" s="4"/>
       <c r="N100" s="4"/>
-      <c r="O100" s="4"/>
-    </row>
-    <row r="101" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>116</v>
       </c>
@@ -4565,33 +4457,31 @@
       <c r="I101" s="4"/>
       <c r="J101" s="4"/>
       <c r="K101" s="4"/>
-      <c r="L101" s="4"/>
-      <c r="M101" s="4">
-        <v>0</v>
-      </c>
+      <c r="L101" s="4">
+        <v>0</v>
+      </c>
+      <c r="M101" s="4"/>
       <c r="N101" s="4"/>
-      <c r="O101" s="4"/>
-    </row>
-    <row r="102" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="9" t="s">
+    </row>
+    <row r="102" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B102" s="9"/>
-      <c r="C102" s="9"/>
-      <c r="D102" s="9"/>
-      <c r="E102" s="9"/>
-      <c r="F102" s="9"/>
-      <c r="G102" s="9"/>
-      <c r="H102" s="9"/>
-      <c r="I102" s="9"/>
-      <c r="J102" s="9"/>
-      <c r="K102" s="9"/>
-      <c r="L102" s="9"/>
-      <c r="M102" s="9"/>
-      <c r="N102" s="9"/>
-      <c r="O102" s="9"/>
-    </row>
-    <row r="103" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="6"/>
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="6"/>
+      <c r="K102" s="6"/>
+      <c r="L102" s="6"/>
+      <c r="M102" s="6"/>
+      <c r="N102" s="6"/>
+    </row>
+    <row r="103" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>117</v>
       </c>
@@ -4619,14 +4509,13 @@
       <c r="I103" s="4"/>
       <c r="J103" s="4"/>
       <c r="K103" s="4"/>
-      <c r="L103" s="4"/>
-      <c r="M103" s="4">
-        <v>0</v>
-      </c>
+      <c r="L103" s="4">
+        <v>0</v>
+      </c>
+      <c r="M103" s="4"/>
       <c r="N103" s="4"/>
-      <c r="O103" s="4"/>
-    </row>
-    <row r="104" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>118</v>
       </c>
@@ -4654,14 +4543,13 @@
       <c r="I104" s="4"/>
       <c r="J104" s="4"/>
       <c r="K104" s="4"/>
-      <c r="L104" s="4"/>
-      <c r="M104" s="4">
-        <v>0</v>
-      </c>
+      <c r="L104" s="4">
+        <v>0</v>
+      </c>
+      <c r="M104" s="4"/>
       <c r="N104" s="4"/>
-      <c r="O104" s="4"/>
-    </row>
-    <row r="105" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>119</v>
       </c>
@@ -4689,14 +4577,13 @@
       <c r="I105" s="4"/>
       <c r="J105" s="4"/>
       <c r="K105" s="4"/>
-      <c r="L105" s="4"/>
-      <c r="M105" s="4">
-        <v>0</v>
-      </c>
+      <c r="L105" s="4">
+        <v>0</v>
+      </c>
+      <c r="M105" s="4"/>
       <c r="N105" s="4"/>
-      <c r="O105" s="4"/>
-    </row>
-    <row r="106" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>120</v>
       </c>
@@ -4724,14 +4611,13 @@
       <c r="I106" s="4"/>
       <c r="J106" s="4"/>
       <c r="K106" s="4"/>
-      <c r="L106" s="4"/>
-      <c r="M106" s="4">
-        <v>0</v>
-      </c>
+      <c r="L106" s="4">
+        <v>0</v>
+      </c>
+      <c r="M106" s="4"/>
       <c r="N106" s="4"/>
-      <c r="O106" s="4"/>
-    </row>
-    <row r="107" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>121</v>
       </c>
@@ -4759,14 +4645,13 @@
       <c r="I107" s="4"/>
       <c r="J107" s="4"/>
       <c r="K107" s="4"/>
-      <c r="L107" s="4"/>
-      <c r="M107" s="4">
-        <v>0</v>
-      </c>
+      <c r="L107" s="4">
+        <v>0</v>
+      </c>
+      <c r="M107" s="4"/>
       <c r="N107" s="4"/>
-      <c r="O107" s="4"/>
-    </row>
-    <row r="108" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>122</v>
       </c>
@@ -4794,14 +4679,13 @@
       <c r="I108" s="4"/>
       <c r="J108" s="4"/>
       <c r="K108" s="4"/>
-      <c r="L108" s="4"/>
-      <c r="M108" s="4">
-        <v>0</v>
-      </c>
+      <c r="L108" s="4">
+        <v>0</v>
+      </c>
+      <c r="M108" s="4"/>
       <c r="N108" s="4"/>
-      <c r="O108" s="4"/>
-    </row>
-    <row r="109" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>123</v>
       </c>
@@ -4829,33 +4713,31 @@
       <c r="I109" s="4"/>
       <c r="J109" s="4"/>
       <c r="K109" s="4"/>
-      <c r="L109" s="4"/>
-      <c r="M109" s="4">
-        <v>0</v>
-      </c>
+      <c r="L109" s="4">
+        <v>0</v>
+      </c>
+      <c r="M109" s="4"/>
       <c r="N109" s="4"/>
-      <c r="O109" s="4"/>
-    </row>
-    <row r="110" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="9" t="s">
+    </row>
+    <row r="110" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B110" s="9"/>
-      <c r="C110" s="9"/>
-      <c r="D110" s="9"/>
-      <c r="E110" s="9"/>
-      <c r="F110" s="9"/>
-      <c r="G110" s="9"/>
-      <c r="H110" s="9"/>
-      <c r="I110" s="9"/>
-      <c r="J110" s="9"/>
-      <c r="K110" s="9"/>
-      <c r="L110" s="9"/>
-      <c r="M110" s="9"/>
-      <c r="N110" s="9"/>
-      <c r="O110" s="9"/>
-    </row>
-    <row r="111" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="6"/>
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6"/>
+      <c r="F110" s="6"/>
+      <c r="G110" s="6"/>
+      <c r="H110" s="6"/>
+      <c r="I110" s="6"/>
+      <c r="J110" s="6"/>
+      <c r="K110" s="6"/>
+      <c r="L110" s="6"/>
+      <c r="M110" s="6"/>
+      <c r="N110" s="6"/>
+    </row>
+    <row r="111" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>124</v>
       </c>
@@ -4883,14 +4765,13 @@
       <c r="I111" s="4"/>
       <c r="J111" s="4"/>
       <c r="K111" s="4"/>
-      <c r="L111" s="4"/>
-      <c r="M111" s="4">
-        <v>0</v>
-      </c>
+      <c r="L111" s="4">
+        <v>0</v>
+      </c>
+      <c r="M111" s="4"/>
       <c r="N111" s="4"/>
-      <c r="O111" s="4"/>
-    </row>
-    <row r="112" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>126</v>
       </c>
@@ -4918,14 +4799,13 @@
       <c r="I112" s="4"/>
       <c r="J112" s="4"/>
       <c r="K112" s="4"/>
-      <c r="L112" s="4"/>
-      <c r="M112" s="4">
-        <v>0</v>
-      </c>
+      <c r="L112" s="4">
+        <v>0</v>
+      </c>
+      <c r="M112" s="4"/>
       <c r="N112" s="4"/>
-      <c r="O112" s="4"/>
-    </row>
-    <row r="113" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>127</v>
       </c>
@@ -4953,14 +4833,13 @@
       <c r="I113" s="4"/>
       <c r="J113" s="4"/>
       <c r="K113" s="4"/>
-      <c r="L113" s="4"/>
-      <c r="M113" s="4">
-        <v>0</v>
-      </c>
+      <c r="L113" s="4">
+        <v>0</v>
+      </c>
+      <c r="M113" s="4"/>
       <c r="N113" s="4"/>
-      <c r="O113" s="4"/>
-    </row>
-    <row r="114" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>128</v>
       </c>
@@ -4988,16 +4867,15 @@
       <c r="I114" s="4"/>
       <c r="J114" s="4"/>
       <c r="K114" s="4"/>
-      <c r="L114" s="4"/>
-      <c r="M114" s="4">
+      <c r="L114" s="4">
         <v>4</v>
       </c>
-      <c r="N114" s="4"/>
-      <c r="O114" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="115" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M114" s="4"/>
+      <c r="N114" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>129</v>
       </c>
@@ -5025,16 +4903,15 @@
       <c r="I115" s="4"/>
       <c r="J115" s="4"/>
       <c r="K115" s="4"/>
-      <c r="L115" s="4"/>
-      <c r="M115" s="4">
-        <v>1</v>
-      </c>
-      <c r="N115" s="4"/>
-      <c r="O115" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="116" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L115" s="4">
+        <v>1</v>
+      </c>
+      <c r="M115" s="4"/>
+      <c r="N115" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>130</v>
       </c>
@@ -5062,14 +4939,13 @@
       <c r="I116" s="4"/>
       <c r="J116" s="4"/>
       <c r="K116" s="4"/>
-      <c r="L116" s="4"/>
-      <c r="M116" s="4">
-        <v>0</v>
-      </c>
+      <c r="L116" s="4">
+        <v>0</v>
+      </c>
+      <c r="M116" s="4"/>
       <c r="N116" s="4"/>
-      <c r="O116" s="4"/>
-    </row>
-    <row r="117" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>131</v>
       </c>
@@ -5095,33 +4971,31 @@
       <c r="I117" s="4"/>
       <c r="J117" s="4"/>
       <c r="K117" s="4"/>
-      <c r="L117" s="4"/>
-      <c r="M117" s="4">
-        <v>0</v>
-      </c>
+      <c r="L117" s="4">
+        <v>0</v>
+      </c>
+      <c r="M117" s="4"/>
       <c r="N117" s="4"/>
-      <c r="O117" s="4"/>
-    </row>
-    <row r="118" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="9" t="s">
+    </row>
+    <row r="118" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B118" s="9"/>
-      <c r="C118" s="9"/>
-      <c r="D118" s="9"/>
-      <c r="E118" s="9"/>
-      <c r="F118" s="9"/>
-      <c r="G118" s="9"/>
-      <c r="H118" s="9"/>
-      <c r="I118" s="9"/>
-      <c r="J118" s="9"/>
-      <c r="K118" s="9"/>
-      <c r="L118" s="9"/>
-      <c r="M118" s="9"/>
-      <c r="N118" s="9"/>
-      <c r="O118" s="9"/>
-    </row>
-    <row r="119" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B118" s="6"/>
+      <c r="C118" s="6"/>
+      <c r="D118" s="6"/>
+      <c r="E118" s="6"/>
+      <c r="F118" s="6"/>
+      <c r="G118" s="6"/>
+      <c r="H118" s="6"/>
+      <c r="I118" s="6"/>
+      <c r="J118" s="6"/>
+      <c r="K118" s="6"/>
+      <c r="L118" s="6"/>
+      <c r="M118" s="6"/>
+      <c r="N118" s="6"/>
+    </row>
+    <row r="119" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>132</v>
       </c>
@@ -5149,18 +5023,17 @@
       <c r="I119" s="4"/>
       <c r="J119" s="4"/>
       <c r="K119" s="4"/>
-      <c r="L119" s="4"/>
+      <c r="L119" s="4">
+        <v>5</v>
+      </c>
       <c r="M119" s="4">
-        <v>5</v>
-      </c>
-      <c r="N119" s="4">
-        <v>1</v>
-      </c>
-      <c r="O119" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="120" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N119" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>133</v>
       </c>
@@ -5188,14 +5061,13 @@
       <c r="I120" s="4"/>
       <c r="J120" s="4"/>
       <c r="K120" s="4"/>
-      <c r="L120" s="4"/>
-      <c r="M120" s="4">
-        <v>0</v>
-      </c>
+      <c r="L120" s="4">
+        <v>0</v>
+      </c>
+      <c r="M120" s="4"/>
       <c r="N120" s="4"/>
-      <c r="O120" s="4"/>
-    </row>
-    <row r="121" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>134</v>
       </c>
@@ -5221,28 +5093,25 @@
         <v>1</v>
       </c>
       <c r="I121" s="4">
+        <v>180</v>
+      </c>
+      <c r="J121" s="4">
+        <v>-30</v>
+      </c>
+      <c r="K121" s="4">
+        <v>225</v>
+      </c>
+      <c r="L121" s="4">
         <v>5</v>
       </c>
-      <c r="J121" s="4">
-        <v>180</v>
-      </c>
-      <c r="K121" s="4">
-        <v>-30</v>
-      </c>
-      <c r="L121" s="4">
-        <v>225</v>
-      </c>
       <c r="M121" s="4">
-        <v>5</v>
-      </c>
-      <c r="N121" s="4">
-        <v>1</v>
-      </c>
-      <c r="O121" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="122" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N121" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>135</v>
       </c>
@@ -5270,14 +5139,13 @@
       <c r="I122" s="4"/>
       <c r="J122" s="4"/>
       <c r="K122" s="4"/>
-      <c r="L122" s="4"/>
-      <c r="M122" s="4">
-        <v>0</v>
-      </c>
+      <c r="L122" s="4">
+        <v>0</v>
+      </c>
+      <c r="M122" s="4"/>
       <c r="N122" s="4"/>
-      <c r="O122" s="4"/>
-    </row>
-    <row r="123" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>136</v>
       </c>
@@ -5303,18 +5171,17 @@
       <c r="I123" s="4"/>
       <c r="J123" s="4"/>
       <c r="K123" s="4"/>
-      <c r="L123" s="4"/>
+      <c r="L123" s="4">
+        <v>5</v>
+      </c>
       <c r="M123" s="4">
-        <v>5</v>
-      </c>
-      <c r="N123" s="4">
-        <v>1</v>
-      </c>
-      <c r="O123" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="124" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N123" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>137</v>
       </c>
@@ -5340,14 +5207,13 @@
       <c r="I124" s="4"/>
       <c r="J124" s="4"/>
       <c r="K124" s="4"/>
-      <c r="L124" s="4"/>
-      <c r="M124" s="4">
-        <v>0</v>
-      </c>
+      <c r="L124" s="4">
+        <v>0</v>
+      </c>
+      <c r="M124" s="4"/>
       <c r="N124" s="4"/>
-      <c r="O124" s="4"/>
-    </row>
-    <row r="125" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>138</v>
       </c>
@@ -5373,14 +5239,13 @@
       <c r="I125" s="4"/>
       <c r="J125" s="4"/>
       <c r="K125" s="4"/>
-      <c r="L125" s="4"/>
-      <c r="M125" s="4">
-        <v>0</v>
-      </c>
+      <c r="L125" s="4">
+        <v>0</v>
+      </c>
+      <c r="M125" s="4"/>
       <c r="N125" s="4"/>
-      <c r="O125" s="4"/>
-    </row>
-    <row r="126" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>139</v>
       </c>
@@ -5408,25 +5273,24 @@
       <c r="I126" s="4"/>
       <c r="J126" s="4"/>
       <c r="K126" s="4"/>
-      <c r="L126" s="4"/>
+      <c r="L126" s="4">
+        <v>5</v>
+      </c>
       <c r="M126" s="4">
-        <v>5</v>
-      </c>
-      <c r="N126" s="4">
-        <v>1</v>
-      </c>
-      <c r="O126" s="4" t="s">
-        <v>157</v>
+        <v>1</v>
+      </c>
+      <c r="N126" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A118:O118"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A31:O31"/>
-    <mergeCell ref="A98:O98"/>
-    <mergeCell ref="A102:O102"/>
-    <mergeCell ref="A110:O110"/>
+    <mergeCell ref="A118:N118"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A31:N31"/>
+    <mergeCell ref="A98:N98"/>
+    <mergeCell ref="A102:N102"/>
+    <mergeCell ref="A110:N110"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>